<commit_message>
fix excel reading one more time
</commit_message>
<xml_diff>
--- a/tests/timetable.xlsx
+++ b/tests/timetable.xlsx
@@ -66,7 +66,7 @@
     <t>Спортзал</t>
   </si>
   <si>
-    <t>10-4</t>
+    <t>10.4</t>
   </si>
 </sst>
 </file>
@@ -107,13 +107,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -406,17 +406,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+      <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -456,10 +456,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -470,8 +470,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
@@ -494,10 +494,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -508,8 +508,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>